<commit_message>
Nuevo formato de subida de tiendas.
</commit_message>
<xml_diff>
--- a/public/uploads/formats/stores_charge.xlsx
+++ b/public/uploads/formats/stores_charge.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzioperez/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzioperez/Desarrollo/Proyectos/backend-regalalo/public/uploads/formats/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDB2454-6F07-3A4E-B3F7-4CB1C308F821}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="27200" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="2060" yWindow="3100" windowWidth="27200" windowHeight="14900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Razón social</t>
   </si>
@@ -105,12 +106,21 @@
   </si>
   <si>
     <t>URL de la Tienda</t>
+  </si>
+  <si>
+    <t>Adquirier ID</t>
+  </si>
+  <si>
+    <t>Wallet Password</t>
+  </si>
+  <si>
+    <t>Gateway Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -128,12 +138,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -148,12 +164,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,6 +180,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -430,11 +450,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,80 +473,83 @@
     <col min="15" max="15" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13" customWidth="1"/>
+    <col min="23" max="23" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="2" t="s">
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="M2" t="s">
@@ -551,12 +574,21 @@
         <v>23</v>
       </c>
       <c r="T2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="R1:V1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:E1"/>

</xml_diff>